<commit_message>
Motor driver STM pin assignment replacement
</commit_message>
<xml_diff>
--- a/Productions/UGOKU-One_V0.42_BOM.xlsx
+++ b/Productions/UGOKU-One_V0.42_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA\Documents\KiCad\MultiBoardMini_HW\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA2\Documents\KiCad\UGOKU-One\Productions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4DFB47-9332-46B2-88C3-E011ACC065D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E0A2D3-9F3C-4452-A66B-FA9CE15957CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="0" windowWidth="21585" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Update Diode footprint and servo pin header
</commit_message>
<xml_diff>
--- a/Productions/UGOKU-One_V0.42_BOM.xlsx
+++ b/Productions/UGOKU-One_V0.42_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TA2\Documents\KiCad\UGOKU-One\Productions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E0A2D3-9F3C-4452-A66B-FA9CE15957CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3155A9-2A46-49B2-B2E1-78A00A5F741A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="0" windowWidth="21585" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>Comment</t>
   </si>
@@ -178,10 +178,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>C2844302</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>3.3uF</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -205,11 +201,112 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>ESP32-WROOM-32</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>ESP32-WROOM-32E-N16</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>TB67H303HG</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C2182175</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C1556864</t>
+  </si>
+  <si>
+    <t>A2541HWV-4P</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>B-2200S15P-A120</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>PZ254V-12-6P</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>B03B-XASK-1-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>B04B-XASK-1(LF)(SN)</t>
+  </si>
+  <si>
+    <t>A2541WV-3P</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>U4,U5</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>T1,T2,T3</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>J4</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CN1,CN2,CN3</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CN4</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>J6</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>P1,P2</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C124408</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C5176037</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C264992</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C264994</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C5333416</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C492420</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>C3032345</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Diode</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>SOD-123F</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -261,12 +358,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -298,7 +401,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -325,6 +428,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,76 +570,16 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="ユーザー定義 3">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
-        <a:ea typeface=""/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Yu Gothic UI"/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Yu Gothic UI"/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,18 +727,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="36.125" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="23.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -713,7 +771,7 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
@@ -722,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -730,7 +788,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>2</v>
@@ -742,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>2</v>
@@ -772,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -816,9 +874,15 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -842,7 +906,7 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -873,16 +937,110 @@
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>41</v>
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="5">
+        <v>1792863</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>